<commit_message>
g8.3 - reestruturação para evitar evitar de referência
</commit_message>
<xml_diff>
--- a/Data/g8.3.xlsx
+++ b/Data/g8.3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,12 +441,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>2025-2024</t>
+          <t>Categoria</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>2025/1997</t>
+          <t>Valor</t>
         </is>
       </c>
     </row>
@@ -456,11 +456,13 @@
           <t>Gás-BR</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-2024</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>-35.24428059585877</v>
-      </c>
-      <c r="C2" t="n">
-        <v>269.5602310681157</v>
       </c>
     </row>
     <row r="3">
@@ -469,11 +471,13 @@
           <t>Gás-NE</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-2024</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>-43.81402676005936</v>
-      </c>
-      <c r="C3" t="n">
-        <v>-54.68498494151564</v>
       </c>
     </row>
     <row r="4">
@@ -482,11 +486,13 @@
           <t>Gás-SE</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-2024</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>-38.07047593582452</v>
-      </c>
-      <c r="C4" t="n">
-        <v>-98.15290549268987</v>
       </c>
     </row>
     <row r="5">
@@ -495,11 +501,13 @@
           <t>LGN-BR</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2025-2024</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
         <v>-44.07929141415514</v>
-      </c>
-      <c r="C5" t="n">
-        <v>52.62759760343716</v>
       </c>
     </row>
     <row r="6">
@@ -508,11 +516,13 @@
           <t>LGN-NE</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2025-2024</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
         <v>-29.18970863480975</v>
-      </c>
-      <c r="C6" t="n">
-        <v>-86.42868143611607</v>
       </c>
     </row>
     <row r="7">
@@ -521,10 +531,12 @@
           <t>LGN-SE</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="n">
-        <v>-100</v>
-      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2025-2024</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -532,11 +544,13 @@
           <t>Petróleo-BR</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2025-2024</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
         <v>-36.91842092174158</v>
-      </c>
-      <c r="C8" t="n">
-        <v>153.3741001090112</v>
       </c>
     </row>
     <row r="9">
@@ -545,11 +559,13 @@
           <t>Petróleo-NE</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2025-2024</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
         <v>-37.84140403772091</v>
-      </c>
-      <c r="C9" t="n">
-        <v>-79.12443946814697</v>
       </c>
     </row>
     <row r="10">
@@ -558,10 +574,147 @@
           <t>Petróleo-SE</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2025-2024</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
         <v>-26.48295957781719</v>
       </c>
-      <c r="C10" t="n">
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Gás-BR</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2025/1997</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>269.5602310681157</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Gás-NE</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2025/1997</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>-54.68498494151564</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Gás-SE</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2025/1997</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>-98.15290549268987</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>LGN-BR</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2025/1997</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>52.62759760343716</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>LGN-NE</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2025/1997</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>-86.42868143611607</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>LGN-SE</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2025/1997</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Petróleo-BR</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2025/1997</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>153.3741001090112</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Petróleo-NE</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2025/1997</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>-79.12443946814697</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Petróleo-SE</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2025/1997</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
         <v>-77.64233321010346</v>
       </c>
     </row>

</xml_diff>

<commit_message>
g8.3 - correção nas colunas
</commit_message>
<xml_diff>
--- a/Data/g8.3.xlsx
+++ b/Data/g8.3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,12 +441,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Categoria</t>
+          <t>atual-ano anterior</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>atual/1997</t>
         </is>
       </c>
     </row>
@@ -456,13 +456,11 @@
           <t>Gás-BR</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2025-2024</t>
-        </is>
+      <c r="B2" t="n">
+        <v>-35.24428059585877</v>
       </c>
       <c r="C2" t="n">
-        <v>-35.24428059585877</v>
+        <v>269.5602310681157</v>
       </c>
     </row>
     <row r="3">
@@ -471,13 +469,11 @@
           <t>Gás-NE</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2025-2024</t>
-        </is>
+      <c r="B3" t="n">
+        <v>-43.81402676005936</v>
       </c>
       <c r="C3" t="n">
-        <v>-43.81402676005936</v>
+        <v>-54.68498494151564</v>
       </c>
     </row>
     <row r="4">
@@ -486,13 +482,11 @@
           <t>Gás-SE</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2025-2024</t>
-        </is>
+      <c r="B4" t="n">
+        <v>-38.07047593582452</v>
       </c>
       <c r="C4" t="n">
-        <v>-38.07047593582452</v>
+        <v>-98.15290549268987</v>
       </c>
     </row>
     <row r="5">
@@ -501,13 +495,11 @@
           <t>LGN-BR</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2025-2024</t>
-        </is>
+      <c r="B5" t="n">
+        <v>-44.07929141415514</v>
       </c>
       <c r="C5" t="n">
-        <v>-44.07929141415514</v>
+        <v>52.62759760343716</v>
       </c>
     </row>
     <row r="6">
@@ -516,13 +508,11 @@
           <t>LGN-NE</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2025-2024</t>
-        </is>
+      <c r="B6" t="n">
+        <v>-29.18970863480975</v>
       </c>
       <c r="C6" t="n">
-        <v>-29.18970863480975</v>
+        <v>-86.42868143611607</v>
       </c>
     </row>
     <row r="7">
@@ -531,12 +521,10 @@
           <t>LGN-SE</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2025-2024</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="n">
+        <v>-100</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -544,13 +532,11 @@
           <t>Petróleo-BR</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2025-2024</t>
-        </is>
+      <c r="B8" t="n">
+        <v>-36.91842092174158</v>
       </c>
       <c r="C8" t="n">
-        <v>-36.91842092174158</v>
+        <v>153.3741001090112</v>
       </c>
     </row>
     <row r="9">
@@ -559,13 +545,11 @@
           <t>Petróleo-NE</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2025-2024</t>
-        </is>
+      <c r="B9" t="n">
+        <v>-37.84140403772091</v>
       </c>
       <c r="C9" t="n">
-        <v>-37.84140403772091</v>
+        <v>-79.12443946814697</v>
       </c>
     </row>
     <row r="10">
@@ -574,147 +558,10 @@
           <t>Petróleo-SE</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2025-2024</t>
-        </is>
+      <c r="B10" t="n">
+        <v>-26.48295957781719</v>
       </c>
       <c r="C10" t="n">
-        <v>-26.48295957781719</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Gás-BR</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>2025/1997</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>269.5602310681157</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Gás-NE</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>2025/1997</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>-54.68498494151564</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Gás-SE</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>2025/1997</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>-98.15290549268987</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>LGN-BR</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>2025/1997</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>52.62759760343716</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>LGN-NE</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>2025/1997</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>-86.42868143611607</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>LGN-SE</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>2025/1997</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>-100</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Petróleo-BR</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>2025/1997</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>153.3741001090112</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Petróleo-NE</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>2025/1997</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>-79.12443946814697</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Petróleo-SE</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>2025/1997</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
         <v>-77.64233321010346</v>
       </c>
     </row>

</xml_diff>

<commit_message>
g8.3 - adição de categoria com valores fixos para uso no bi
</commit_message>
<xml_diff>
--- a/Data/g8.3.xlsx
+++ b/Data/g8.3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,12 +441,17 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>atual-ano anterior</t>
+          <t>Período</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>atual/1997</t>
+          <t>Valor</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Categoria</t>
         </is>
       </c>
     </row>
@@ -456,11 +461,18 @@
           <t>Gás-BR</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-2024</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>-35.24428059585877</v>
       </c>
-      <c r="C2" t="n">
-        <v>269.5602310681157</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Variação do último ano</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -469,11 +481,18 @@
           <t>Gás-NE</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-2024</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>-43.81402676005936</v>
       </c>
-      <c r="C3" t="n">
-        <v>-54.68498494151564</v>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Variação do último ano</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -482,11 +501,18 @@
           <t>Gás-SE</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-2024</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>-38.07047593582452</v>
       </c>
-      <c r="C4" t="n">
-        <v>-98.15290549268987</v>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Variação do último ano</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -495,11 +521,18 @@
           <t>LGN-BR</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2025-2024</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
         <v>-44.07929141415514</v>
       </c>
-      <c r="C5" t="n">
-        <v>52.62759760343716</v>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Variação do último ano</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -508,11 +541,18 @@
           <t>LGN-NE</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2025-2024</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
         <v>-29.18970863480975</v>
       </c>
-      <c r="C6" t="n">
-        <v>-86.42868143611607</v>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Variação do último ano</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -521,9 +561,16 @@
           <t>LGN-SE</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="n">
-        <v>-100</v>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2025-2024</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Variação do último ano</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -532,11 +579,18 @@
           <t>Petróleo-BR</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2025-2024</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
         <v>-36.91842092174158</v>
       </c>
-      <c r="C8" t="n">
-        <v>153.3741001090112</v>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Variação do último ano</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -545,11 +599,18 @@
           <t>Petróleo-NE</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2025-2024</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
         <v>-37.84140403772091</v>
       </c>
-      <c r="C9" t="n">
-        <v>-79.12443946814697</v>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Variação do último ano</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -558,11 +619,198 @@
           <t>Petróleo-SE</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2025-2024</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
         <v>-26.48295957781719</v>
       </c>
-      <c r="C10" t="n">
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Variação do último ano</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Gás-BR</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2025/1997</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>269.5602310681157</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Variação desde 1997</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Gás-NE</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2025/1997</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>-54.68498494151564</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Variação desde 1997</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Gás-SE</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2025/1997</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>-98.15290549268987</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Variação desde 1997</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>LGN-BR</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2025/1997</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>52.62759760343716</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Variação desde 1997</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>LGN-NE</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2025/1997</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>-86.42868143611607</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Variação desde 1997</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>LGN-SE</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2025/1997</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>-100</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Variação desde 1997</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Petróleo-BR</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2025/1997</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>153.3741001090112</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Variação desde 1997</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Petróleo-NE</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2025/1997</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>-79.12443946814697</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Variação desde 1997</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Petróleo-SE</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2025/1997</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
         <v>-77.64233321010346</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Variação desde 1997</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>